<commit_message>
ERD modified: minor change to mall, a table added for customers
</commit_message>
<xml_diff>
--- a/남근우 일정표.xlsx
+++ b/남근우 일정표.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t xml:space="preserve">4월</t>
   </si>
@@ -60,6 +60,12 @@
   </si>
   <si>
     <t xml:space="preserve">오류 수정 및 추가기능 구현</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5주차 한 일</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DB 수정: 맵 사이즈의 최대 저장 크기 증가</t>
   </si>
 </sst>
 </file>
@@ -185,7 +191,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -223,10 +229,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -322,7 +324,7 @@
   </sheetPr>
   <dimension ref="A1:N9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H6" activeCellId="0" sqref="H6"/>
     </sheetView>
   </sheetViews>
@@ -407,15 +409,15 @@
       <c r="E3" s="7"/>
       <c r="F3" s="8"/>
       <c r="G3" s="9"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="11" t="s">
+      <c r="H3" s="5"/>
+      <c r="I3" s="10" t="s">
         <v>5</v>
       </c>
       <c r="J3" s="8"/>
       <c r="K3" s="8"/>
       <c r="L3" s="8"/>
       <c r="M3" s="8"/>
-      <c r="N3" s="11" t="s">
+      <c r="N3" s="10" t="s">
         <v>6</v>
       </c>
     </row>
@@ -428,14 +430,14 @@
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
       <c r="F4" s="8"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="10"/>
       <c r="J4" s="8"/>
       <c r="K4" s="8"/>
       <c r="L4" s="8"/>
       <c r="M4" s="8"/>
-      <c r="N4" s="11"/>
+      <c r="N4" s="10"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5"/>
@@ -445,14 +447,14 @@
       <c r="C5" s="7"/>
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="11"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="10"/>
       <c r="J5" s="6"/>
       <c r="K5" s="8"/>
       <c r="L5" s="8"/>
       <c r="M5" s="8"/>
-      <c r="N5" s="11"/>
+      <c r="N5" s="10"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5"/>
@@ -462,14 +464,14 @@
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
       <c r="F6" s="6"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="11"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="10"/>
       <c r="J6" s="6"/>
       <c r="K6" s="6"/>
       <c r="L6" s="8"/>
       <c r="M6" s="8"/>
-      <c r="N6" s="11"/>
+      <c r="N6" s="10"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5"/>
@@ -480,14 +482,14 @@
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
       <c r="F7" s="8"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="10"/>
       <c r="J7" s="6"/>
       <c r="K7" s="6"/>
       <c r="L7" s="8"/>
       <c r="M7" s="8"/>
-      <c r="N7" s="11"/>
+      <c r="N7" s="10"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5"/>
@@ -498,14 +500,14 @@
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="10"/>
       <c r="J8" s="7"/>
       <c r="K8" s="6"/>
       <c r="L8" s="6"/>
       <c r="M8" s="6"/>
-      <c r="N8" s="11"/>
+      <c r="N8" s="10"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -535,17 +537,28 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.6"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>